<commit_message>
update and bug fixs
signuter update, 
bug fix energy carrier names with spaces, 
update cm category
update solar thermal constraint
</commit_message>
<xml_diff>
--- a/cm/tests/data/INPUTS_CALCULATION_MODULE.xlsx
+++ b/cm/tests/data/INPUTS_CALCULATION_MODULE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20348"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C396873-ADDB-4B3D-9B06-65A0ABF82F9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFBA437-7B96-473E-8040-23F57B4513A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{A39C18F9-790E-4AC0-B0AE-6D70F2BE89C8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="135">
   <si>
     <t>input_name</t>
   </si>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED82753-5272-4518-B7D2-E7729D132D1F}">
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,9 +863,7 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -889,9 +887,7 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -915,9 +911,7 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -941,9 +935,7 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -967,9 +959,7 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1250,12 +1240,8 @@
       <c r="F17" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1276,12 +1262,8 @@
       <c r="F18" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1302,12 +1284,8 @@
       <c r="F19" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1328,12 +1306,8 @@
       <c r="F20" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1354,12 +1328,8 @@
       <c r="F21" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1383,9 +1353,7 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1409,9 +1377,7 @@
       <c r="G23" s="1">
         <v>0</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1435,9 +1401,7 @@
       <c r="G24" s="1">
         <v>0</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1461,9 +1425,7 @@
       <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1487,9 +1449,7 @@
       <c r="G26" s="1">
         <v>0</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1513,9 +1473,7 @@
       <c r="G27" s="1">
         <v>0</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1539,9 +1497,7 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1565,9 +1521,7 @@
       <c r="G29" s="1">
         <v>0</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1591,9 +1545,7 @@
       <c r="G30" s="1">
         <v>0</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1617,9 +1569,7 @@
       <c r="G31" s="1">
         <v>0</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1643,9 +1593,7 @@
       <c r="G32" s="1">
         <v>0</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1669,9 +1617,7 @@
       <c r="G33" s="1">
         <v>0</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1695,9 +1641,7 @@
       <c r="G34" s="1">
         <v>0</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1721,9 +1665,7 @@
       <c r="G35" s="1">
         <v>0</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1747,9 +1689,7 @@
       <c r="G36" s="1">
         <v>0</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1900,12 +1840,8 @@
       <c r="F42" t="s">
         <v>49</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1926,12 +1862,8 @@
       <c r="F43" t="s">
         <v>49</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1952,12 +1884,8 @@
       <c r="F44" t="s">
         <v>49</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1978,12 +1906,8 @@
       <c r="F45" t="s">
         <v>49</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -2004,12 +1928,8 @@
       <c r="F46" t="s">
         <v>49</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -2030,12 +1950,8 @@
       <c r="F47" t="s">
         <v>49</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -2056,12 +1972,8 @@
       <c r="F48" t="s">
         <v>81</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -2082,12 +1994,8 @@
       <c r="F49" t="s">
         <v>81</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -2108,12 +2016,8 @@
       <c r="F50" t="s">
         <v>81</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -2134,12 +2038,8 @@
       <c r="F51" t="s">
         <v>81</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -2160,12 +2060,8 @@
       <c r="F52" t="s">
         <v>81</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -2186,12 +2082,8 @@
       <c r="F53" t="s">
         <v>81</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -2212,12 +2104,8 @@
       <c r="F54" t="s">
         <v>83</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">

</xml_diff>

<commit_message>
show error message if predefined capacities are higher than upper limit
+ new test
</commit_message>
<xml_diff>
--- a/cm/tests/data/INPUTS_CALCULATION_MODULE.xlsx
+++ b/cm/tests/data/INPUTS_CALCULATION_MODULE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20358"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20359"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F830EF3B-5063-4453-8B31-B43B62138EE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CECC5B-096B-47DF-9D5C-66B6201F0495}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1815" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="3015" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,37 +463,37 @@
     <t>EUR/(MW*yr)</t>
   </si>
   <si>
+    <t>wood pellets</t>
+  </si>
+  <si>
+    <t>waste</t>
+  </si>
+  <si>
+    <t>bio gas</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>radiation</t>
+  </si>
+  <si>
+    <t>fix</t>
+  </si>
+  <si>
+    <t>fx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district heating demand </t>
+  </si>
+  <si>
+    <t>dh_demand</t>
+  </si>
+  <si>
+    <t>MWh</t>
+  </si>
+  <si>
     <t>invest</t>
-  </si>
-  <si>
-    <t>wood pellets</t>
-  </si>
-  <si>
-    <t>waste</t>
-  </si>
-  <si>
-    <t>bio gas</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>radiation</t>
-  </si>
-  <si>
-    <t>fix</t>
-  </si>
-  <si>
-    <t>fx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">district heating demand </t>
-  </si>
-  <si>
-    <t>dh_demand</t>
-  </si>
-  <si>
-    <t>MWh</t>
   </si>
 </sst>
 </file>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1129,7 @@
         <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1437,7 +1437,7 @@
         <v>95</v>
       </c>
       <c r="D22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1454,7 +1454,7 @@
         <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1471,7 +1471,7 @@
         <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1488,7 +1488,7 @@
         <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1505,7 +1505,7 @@
         <v>99</v>
       </c>
       <c r="D26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1808,7 +1808,7 @@
         <v>111</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -1851,7 +1851,7 @@
         <v>113</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -1894,7 +1894,7 @@
         <v>115</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -1937,7 +1937,7 @@
         <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -1980,7 +1980,7 @@
         <v>119</v>
       </c>
       <c r="D46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -2023,7 +2023,7 @@
         <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E48">
         <v>2</v>
@@ -2499,22 +2499,22 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>154</v>
+      </c>
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" t="s">
         <v>155</v>
       </c>
-      <c r="B67" t="s">
-        <v>73</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="D67">
+        <v>100000</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" t="s">
         <v>156</v>
-      </c>
-      <c r="D67">
-        <v>100</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67" t="s">
-        <v>157</v>
       </c>
       <c r="G67">
         <v>0</v>

</xml_diff>